<commit_message>
Added Notes folder. changed from 3x5 to 5x5 table corr
Included any notes I've had just to make sure I'm keeping things in one place. Also changed the track comparison to include all 5 tracks against all 5 recorded. May as well
</commit_message>
<xml_diff>
--- a/stats of comparisons.xlsx
+++ b/stats of comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Uni\FINAL_Year\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F08563F-8FCF-4AC3-AD41-BDA44D2357C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261BE0CF-BD62-4858-B3DB-5678A754F8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5293109-9A9A-4D29-9A3D-DCAEEEE50D53}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>NaN</t>
   </si>
@@ -91,10 +91,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D67BC0-35E5-4B63-98F7-F5D0CAA45D67}">
-  <dimension ref="B2:O23"/>
+  <dimension ref="B2:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,19 +420,19 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3.7070252358758299E-2</v>
       </c>
@@ -463,8 +463,38 @@
       <c r="O4">
         <v>4.5814457207404402E-2</v>
       </c>
+      <c r="R4">
+        <v>3.7070252358758299E-2</v>
+      </c>
+      <c r="S4">
+        <v>4.52772434201337E-2</v>
+      </c>
+      <c r="T4">
+        <v>4.5222728461540698E-2</v>
+      </c>
+      <c r="U4">
+        <v>5.7142550395801399E-2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0.109091352958283</v>
+      </c>
+      <c r="AB4">
+        <v>3.9237029185265802E-2</v>
+      </c>
+      <c r="AC4">
+        <v>9.7361990172002102E-2</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>4.5814457207404402E-2</v>
+      </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2.9599108814027698E-2</v>
       </c>
@@ -480,11 +510,11 @@
       <c r="F5">
         <v>1.9007609762988601E-2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="1"/>
       <c r="K5">
         <v>3.2399184106931697E-2</v>
       </c>
@@ -500,8 +530,43 @@
       <c r="O5">
         <v>2.87509407118503E-2</v>
       </c>
+      <c r="R5">
+        <v>2.9599108814027698E-2</v>
+      </c>
+      <c r="S5">
+        <v>0.28981213350422802</v>
+      </c>
+      <c r="T5">
+        <v>5.0893826011012201E-2</v>
+      </c>
+      <c r="U5">
+        <v>1.8923125756805399E-2</v>
+      </c>
+      <c r="V5">
+        <v>1.9007609762988601E-2</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5">
+        <v>3.2399184106931697E-2</v>
+      </c>
+      <c r="AB5">
+        <v>0.18674436428435601</v>
+      </c>
+      <c r="AC5">
+        <v>5.7154397418480003E-2</v>
+      </c>
+      <c r="AD5">
+        <v>3.8034669306380997E-2</v>
+      </c>
+      <c r="AE5">
+        <v>2.87509407118503E-2</v>
+      </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2.6138444125195899E-2</v>
       </c>
@@ -532,8 +597,38 @@
       <c r="O6">
         <v>4.7758533186458098E-2</v>
       </c>
+      <c r="R6">
+        <v>2.6138444125195899E-2</v>
+      </c>
+      <c r="S6">
+        <v>9.4496008984368995E-2</v>
+      </c>
+      <c r="T6">
+        <v>0.34809040457825702</v>
+      </c>
+      <c r="U6">
+        <v>1.8842004493847899E-2</v>
+      </c>
+      <c r="V6">
+        <v>4.0359155621385798E-2</v>
+      </c>
+      <c r="AA6">
+        <v>7.3124911326957698E-2</v>
+      </c>
+      <c r="AB6">
+        <v>0.106038040678218</v>
+      </c>
+      <c r="AC6">
+        <v>0.42445837538753001</v>
+      </c>
+      <c r="AD6">
+        <v>3.9552059312990197E-2</v>
+      </c>
+      <c r="AE6">
+        <v>4.7758533186458098E-2</v>
+      </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7.0429878195652607E-2</v>
       </c>
@@ -565,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.9809100053817402E-2</v>
       </c>
@@ -581,11 +676,11 @@
       <c r="F10">
         <v>1.1968911471256199E-2</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1"/>
       <c r="K10">
         <v>2.1295199825766099E-2</v>
       </c>
@@ -602,7 +697,7 @@
         <v>2.46961442691053E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1.8851670816816799E-2</v>
       </c>
@@ -634,17 +729,17 @@
         <v>3.3693680446220502E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>IF(B9&gt;=B4,B9-B4,B4-B9)</f>
         <v>3.3359625836894308E-2</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="C15:F15" si="0">IF(E9&gt;=E4,E9-E4,E4-E9)</f>
+        <f t="shared" ref="E15" si="0">IF(E9&gt;=E4,E9-E4,E4-E9)</f>
         <v>2.0419089608901597E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="G15:O15" si="1">IF(K9&gt;=K4,K9-K4,K4-K9)</f>
+        <f t="shared" ref="K15:M15" si="1">IF(K9&gt;=K4,K9-K4,K4-K9)</f>
         <v>4.8868585418021096E-2</v>
       </c>
       <c r="M15">
@@ -652,7 +747,7 @@
         <v>4.8520771280213905E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" ref="B16:F17" si="2">IF(B10&gt;=B5,B10-B5,B5-B10)</f>
         <v>9.7900087602102968E-3</v>
@@ -673,12 +768,12 @@
         <f t="shared" si="2"/>
         <v>7.0386982917324016E-3</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="2"/>
       <c r="K16">
-        <f t="shared" ref="G16:O16" si="3">IF(K10&gt;=K5,K10-K5,K5-K10)</f>
+        <f t="shared" ref="K16:O16" si="3">IF(K10&gt;=K5,K10-K5,K5-K10)</f>
         <v>1.1103984281165599E-2</v>
       </c>
       <c r="L16">
@@ -716,7 +811,7 @@
         <v>1.6295370373156995E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="G17:O17" si="4">IF(K11&gt;=K6,K11-K6,K6-K11)</f>
+        <f t="shared" ref="K17:O17" si="4">IF(K11&gt;=K6,K11-K6,K6-K11)</f>
         <v>2.9530096481962947E-3</v>
       </c>
       <c r="L17">
@@ -750,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
+        <f>E15*100</f>
         <v>2.0419089608901597</v>
       </c>
       <c r="F21">
@@ -799,10 +894,10 @@
         <f t="shared" si="6"/>
         <v>0.70386982917324015</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="2"/>
       <c r="K22">
         <f t="shared" si="6"/>
         <v>1.1103984281165598</v>
@@ -867,7 +962,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="X5:Y5"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="L2:N2"/>
@@ -876,7 +972,7 @@
     <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:O15 B17:O17 B16:H16 J16:O16">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -888,79 +984,79 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F6">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:F11">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:O6">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:O11">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:F11">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:O6">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9:O11">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
@@ -968,7 +1064,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:O17">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -978,7 +1074,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -988,7 +1084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:F17">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -998,12 +1094,112 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:V6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA4:AE6">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R6">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S6">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T6">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA4:AA6">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB4:AB6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC4:AC6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>